<commit_message>
Completed the implementation of the import function. Test and Function is works - (Task #967)
---
Task #967: Add CostEquipmentWizard
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost/resources/ExcelExportDefaultTemplate.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost/resources/ExcelExportDefaultTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7754AE0-EAB5-4EDD-B1B3-EFB9E95A2BBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EC85BE-9122-49CE-9842-9E866230E170}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14412" windowHeight="6528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14412" windowHeight="6528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t xml:space="preserve"> Structural Element UUID</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Repository Revision</t>
   </si>
   <si>
-    <t>VirSat IO Sheet for Interfaces and InterfaceEnds</t>
-  </si>
-  <si>
     <t>Property</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>Place an image here</t>
-  </si>
-  <si>
     <t>This is an auto generated ICD Document of Virtual Satellite</t>
   </si>
   <si>
@@ -106,6 +100,9 @@
   </si>
   <si>
     <t>Margin %</t>
+  </si>
+  <si>
+    <t>VirSat IO Sheet for CostTypes and CostEquipments</t>
   </si>
 </sst>
 </file>
@@ -453,13 +450,123 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>312775</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>354</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>906102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1C2236A-8470-4320-8001-11DDEBDF0445}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3779520" y="0"/>
+          <a:ext cx="3185514" cy="906102"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3185514</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>928962</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15971A0E-5146-405C-BC5E-C0C880CA6E5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3634740" y="22860"/>
+          <a:ext cx="3185514" cy="906102"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>998221</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7975</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>906102</xdr:rowOff>
     </xdr:to>
@@ -490,58 +597,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2392681" y="0"/>
+          <a:off x="9784081" y="0"/>
           <a:ext cx="3185514" cy="906102"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2209800</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3070860</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>891540</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Grafik 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{881089F5-D627-4A5C-828D-7A88942491F4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9875520" y="30480"/>
-          <a:ext cx="861060" cy="861060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -876,51 +933,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" customWidth="1"/>
     <col min="2" max="2" width="28.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="29"/>
-      <c r="C1" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -994,7 +1049,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -1008,6 +1063,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1016,50 +1072,48 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="29"/>
-      <c r="C1" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1335,6 +1389,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1342,7 +1397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:I3"/>
     </sheetView>
   </sheetViews>
@@ -1359,7 +1414,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="36"/>
@@ -1372,7 +1427,7 @@
     </row>
     <row r="2" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -1385,10 +1440,10 @@
     </row>
     <row r="3" spans="1:11" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -1400,31 +1455,31 @@
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="H4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>27</v>
-      </c>
       <c r="I4" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">

</xml_diff>